<commit_message>
outputting real data from excel
</commit_message>
<xml_diff>
--- a/test_worksheets_manual.xlsx
+++ b/test_worksheets_manual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Person!$A$1:$F$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Person!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">person_id</t>
   </si>
@@ -77,14 +78,21 @@
   </si>
   <si>
     <t xml:space="preserve">last_day_to_withdraw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSY180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AN130704.0807.5W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -160,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +179,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -196,19 +212,19 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.81111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.537037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,16 +278,16 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.61111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.237037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,20 +317,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.6222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,6 +352,26 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>1395954</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>41459</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>41493</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>41466</v>
       </c>
     </row>
   </sheetData>
@@ -361,7 +398,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>